<commit_message>
adding functionality for student status updates
</commit_message>
<xml_diff>
--- a/daily-status/student_activity.xlsx
+++ b/daily-status/student_activity.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,8 +474,151 @@
           <t>- stood and did nothing</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Silas</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>D - dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Zi</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>S++ sat and pooped</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>C- stood but did not pee in cup</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Arturo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ACC - had an accident in underwear</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Emmy</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>11:30</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>S+ sat and peed</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Rip</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1:30</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>S+ sat and peed</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Braxton</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Journee</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>8:30</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>D - dry</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Zi</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>tester</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>